<commit_message>
add okr and tasks to github
</commit_message>
<xml_diff>
--- a/assets/excel/okr.xlsx
+++ b/assets/excel/okr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\OKR_analyze\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756B05EE-0DEA-482F-B2FB-C05FFA3B0A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA33132-5075-4060-8CA1-C26CE044064C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,32 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Key Results</t>
   </si>
   <si>
-    <t>دریافت دیتا از سامانه ارس</t>
-  </si>
-  <si>
-    <t xml:space="preserve">نهایی سازی نحوه ذخیره سازی و بهره برداری از دیتای سامانه های مدیریت راهبرد </t>
-  </si>
-  <si>
-    <t xml:space="preserve">راه اندازی چت بات  اجرای راهبرد </t>
-  </si>
-  <si>
-    <t xml:space="preserve">تهیه برنامه پیاده سازی دستیار هوش مصنوعی در برنامه پیشنهادی </t>
-  </si>
-  <si>
-    <t>پایلوت تحلیل علت معلولی هوشمند در سطح شاخص ها، راهکار و اهداف کارت امتیازی</t>
-  </si>
-  <si>
-    <t>بازبینی داشبوردهای تهیه شده با برنامه استخراج شده</t>
-  </si>
-  <si>
-    <t>مهاجرت به سرورهای جدید</t>
-  </si>
-  <si>
     <t>KR_code</t>
   </si>
   <si>
@@ -73,6 +52,93 @@
   </si>
   <si>
     <t>kr7</t>
+  </si>
+  <si>
+    <t>پیگیری دریافت تایید کارشناسان حوزه ها برای شناسنامه اهداف سطح CXO</t>
+  </si>
+  <si>
+    <t>تهیه شناسنامه شاخص‌های سطح CXO توسط هوش مصنوعی</t>
+  </si>
+  <si>
+    <t>پیگیری دریافت تایید کارشناسان حوزه ها برای شناسنامه شاخص‌های سطح CXO</t>
+  </si>
+  <si>
+    <t>پیگیری ورود عملکرد شاخص های خودکار شده و رفع مشکلات احتمالی</t>
+  </si>
+  <si>
+    <t>آپدیت داشبوردهای مرتبط با شاخص های خودکار شده</t>
+  </si>
+  <si>
+    <t>نهایی سازی شاخص های راهبرد کهکشان</t>
+  </si>
+  <si>
+    <t>تعیین سطح بلوغ شاخص های راهبرد کهکشان</t>
+  </si>
+  <si>
+    <t>ارتقای سطح اتوماسیون شاخص های کهکشان به سطح 5</t>
+  </si>
+  <si>
+    <t>ساخت داشبوردهای مرتبط</t>
+  </si>
+  <si>
+    <t>تهیه سرور در زون مرتبط با دسترسی های مورد نیاز</t>
+  </si>
+  <si>
+    <t>تهیه سخت افزار مورد نیاز</t>
+  </si>
+  <si>
+    <t>تست مدل های زبانی بزرگ متناسب با  نیازمندی یوزکیس‌ها و سخت افزار مرتبط</t>
+  </si>
+  <si>
+    <t xml:space="preserve">راه اندازی مدل(های) زبانی بزرگ </t>
+  </si>
+  <si>
+    <t>تهیه سفر مشتری فرایند برنامه ریزی</t>
+  </si>
+  <si>
+    <t>تهیه لیستی از بخش‌های سفر مشتری برنامه پیشنهادی که قابلیت استفاده از هوش مصنوعی دارند</t>
+  </si>
+  <si>
+    <t>اولویت بندی و زمانبندی اجرای لیست تهیه شده در نتیجه کلیدی R.3.2</t>
+  </si>
+  <si>
+    <t>امکان سنجی چت با اسناد دارای بخش‌های متنوع مانند تصویر و نمودار</t>
+  </si>
+  <si>
+    <t>امکان سنجی چت با اسناد ADL و سایر اسناد راهبردی معتبر مانند GSMA، OVUM، TM Forum</t>
+  </si>
+  <si>
+    <t>kr8</t>
+  </si>
+  <si>
+    <t>kr9</t>
+  </si>
+  <si>
+    <t>kr10</t>
+  </si>
+  <si>
+    <t>kr11</t>
+  </si>
+  <si>
+    <t>kr12</t>
+  </si>
+  <si>
+    <t>kr13</t>
+  </si>
+  <si>
+    <t>kr14</t>
+  </si>
+  <si>
+    <t>kr15</t>
+  </si>
+  <si>
+    <t>kr16</t>
+  </si>
+  <si>
+    <t>kr17</t>
+  </si>
+  <si>
+    <t>kr18</t>
   </si>
 </sst>
 </file>
@@ -95,13 +161,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color rgb="FF000000"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,7 +182,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -123,17 +190,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0095DA"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF0095DA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF0095DA"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF0095DA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0095DA"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF0095DA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF0095DA"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0095DA"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF0095DA"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0095DA"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF0095DA"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0095DA"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,80 +541,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="73.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
+    </row>
+    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>